<commit_message>
Update Elsevier and requirements.txt
</commit_message>
<xml_diff>
--- a/papers_2024_2024_jfe.xlsx
+++ b/papers_2024_2024_jfe.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="98">
   <si>
     <t>title</t>
   </si>
@@ -31,7 +31,10 @@
     <t>cover_date</t>
   </si>
   <si>
-    <t>author</t>
+    <t>author.name</t>
+  </si>
+  <si>
+    <t>authors</t>
   </si>
   <si>
     <t>volume</t>
@@ -97,6 +100,50 @@
     <t>Independent regulators and financial stability evidence from gubernatorial election campaigns in the Progressive Era</t>
   </si>
   <si>
+    <t>Recent theories and narratives highlight the potential role of associative recall in driving overreaction in expectations and market behavior. Based on a simple model, we test this idea through a series of experiments in which news are communicated with memorable contexts. Because the experimental participants predominantly remember those past news that get cued by new information, their beliefs about fundamentals strongly overreact. In a betting market experiment, associative recall translates into overreaction in market prices, which makes realized prices too extreme. Our results highlight the importance of associative memory for beliefs and financial decisions.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+                  We isolate the information channel of peer effects in consumption in a setting that excludes a role for common shocks or social pressure—a spending panel paired with crowdsourced information about anonymous “peers” elicited at different times. Consumers converge to peers’ spending, and more so when peer signals are more informative. Convergence is asymmetric: within 12 months of information provision, overspenders close 17% and underspenders 5% of their gap relative to peers. We exploit the quasi-random assignment to peer groups in an instrumental-variable strategy and implement an experiment for external validity. Our results are consistent with information-based theories of overconsumption.
+               </t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+                  Do negative housing shocks lead to persistent changes in household attitudes toward housing and homeownership? We use the residential destruction of Germany during World War II (WWII) as a quasi-experiment and exploit the reasonably exogenous region-by-cohort variation in destruction exposure. We find that WWII-experiencing cohorts from high destruction regions are significantly less likely to be homeowners decades later, controlling for regional differences and household characteristics. Underlying this effect are changes in household attitudes toward homeownership that also extend to preferences for housing consumption, with little or no support for risk preferences, income and wealth effects, or supply-side factors.
+               </t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+                  To prevent issuers from inflating their share prices, SEC Rule 10b-18 sets price ceilings on share repurchases through open markets. We find that market-structure reforms in the 1990s and 2000s dramatically increased share repurchases because they relaxed constraints on issuers competing with other buyers under price ceilings. The Tick Size Pilot Program, a controlled experiment that partially reversed previous reforms, significantly reduced share repurchases. We estimate that price ceilings and reduced market-structure frictions explain 18% of the secular increase in share repurchases. Meanwhile, these two frictions still exist, which explains why share repurchases have not crowded out dividends entirely.
+               </t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+                  We investigate how access to robo-advisors impacts the financial investment and welfare of less-wealthy investors. We leverage a quasi-experiment where a major U.S. robo-advisor significantly expands access by reducing its account minimum, increasing participation by middle-class investors but not the poor. A benchmark model calibrated to portfolio-level data rationalizes this increase: middle-class investors want sophisticated investing but cannot achieve it themselves. Their welfare rises moderately, driven by advanced features like multi-dimensional glide-paths and additional priced risk factors. Middle-age investors gain three times more than millennials. Our results reveal novel margins of demand for robo-advisors, helping explain their sustained growth.
+               </t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+                  The average total compensation of directors in U.S.-listed companies was $342,030 in 2020, 5.06 times the median household income. Directors set their own pay, giving rise to potential self-dealing. We argue and document that in the presence of self-dealing, external mechanisms such as legal standards act as effective means of governance. Following a landmark Delaware court ruling that subjected director pay to a more stringent legal standard, Delaware-incorporated firms reduced director compensation relative to non-Delaware firms and experienced positive and non-transient stock price reactions. Our results indicate that proper governance of director compensation enhances firm value.
+               </t>
+  </si>
+  <si>
+    <t>We show that firm valuations fell after a key expense became more visible in financial statements. FAS 123-R required firms to deduct option compensation costs from earnings, instead of disclosing them in footnotes. Firms that granted high option pay experienced earnings reductions, while fundamentals remained unchanged. These firms were more likely to miss earnings forecasts, and they experienced recommendation downgrades and valuation declines. Our findings suggest that market participants exhibited limited attention to option costs before FAS 123-R. As we reuse the FAS 123-R natural experiment, we show how one can address confounding channels by integrating reduced-form and structural estimation.</t>
+  </si>
+  <si>
+    <t>This paper studies bank antitrust rules which discontinuously shift bank mergers' competitive impact. The likelihood of mandatory divestiture rises sharply for mergers in markets above a threshold level of concentration, leading to an increase in the number of banks in these markets. Consistent with greater competition, intervention leads to higher deposit rates. Mortgage originations rise by 11%, from both refinancing and purchases. However, small business loan quantities do not change. The effects of intervention do not dissipate over time, and nonbank lenders respond similarly to banks. Overall, antitrust rules can increase bank competition, but relationships protect banks from competitors.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+                  This study shows that firms regard stock price fragility - exposure to non-fundamental demand shocks stemming from the composition of equity ownership - as a salient corporate risk. We model ex ante corporate responses to higher potential for future stock market misvaluation and then empirically document that within firm variation in equity fragility has effects in line with the model: higher fragility raises cash holdings and lowers investment. Multiple natural experiments support a causal interpretation of the results. The results are shown to be more prominent in the face of high uncertainty and financial constraints. The evidence presents a new dimension of how managerial expectations affect corporate policies.
+               </t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+                  Regulatory independence forms a foundation for modern financial systems. The institutions’ value is illuminated by a Progressive Era policy experiment when independent state-bank regulators came under governors’ supervision. Afterwards, bank resolution rates declined during gubernatorial election campaigns for banks supervised by state but not national authorities. This gubernatorial-campaign effect diminished by two orders of magnitude, but did not disappear, after the FDIC became the independent resolver for all insured banks in 1935. In addition, during the Progressive Era, declines in bank resolutions led to declines in business bankruptcy rates, an effect that is not observed in the FDIC era. Our findings indicate regulatory independence can dramatically reduce but may not eliminate politics’ impact on banks and the economy.
+               </t>
+  </si>
+  <si>
     <t>10.1016/j.jfineco.2024.103853</t>
   </si>
   <si>
@@ -220,7 +267,7 @@
     <t>University of California, Irvine</t>
   </si>
   <si>
-    <t>Handelshögskolan i Stockholm; Centre for Economic Policy Research, London; NHH Norwegian School of Economics</t>
+    <t>NHH Norwegian School of Economics; Handelshögskolan i Stockholm; Centre for Economic Policy Research, London</t>
   </si>
   <si>
     <t>California State University, Los Angeles</t>
@@ -245,6 +292,36 @@
   </si>
   <si>
     <t>8</t>
+  </si>
+  <si>
+    <t>103853</t>
+  </si>
+  <si>
+    <t>103858</t>
+  </si>
+  <si>
+    <t>103835</t>
+  </si>
+  <si>
+    <t>103818</t>
+  </si>
+  <si>
+    <t>103829</t>
+  </si>
+  <si>
+    <t>103813</t>
+  </si>
+  <si>
+    <t>103811</t>
+  </si>
+  <si>
+    <t>103797</t>
+  </si>
+  <si>
+    <t>103795</t>
+  </si>
+  <si>
+    <t>103773</t>
   </si>
 </sst>
 </file>
@@ -602,13 +679,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:Q11"/>
+  <dimension ref="A1:R11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:17">
+    <row r="1" spans="1:18">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -660,324 +737,477 @@
       <c r="Q1" s="1" t="s">
         <v>16</v>
       </c>
+      <c r="R1" s="1" t="s">
+        <v>17</v>
+      </c>
     </row>
-    <row r="2" spans="1:17">
+    <row r="2" spans="1:18">
       <c r="A2" t="s">
-        <v>17</v>
+        <v>18</v>
+      </c>
+      <c r="B2" t="s">
+        <v>28</v>
       </c>
       <c r="C2" t="s">
+        <v>38</v>
+      </c>
+      <c r="D2" t="s">
+        <v>48</v>
+      </c>
+      <c r="E2" t="s">
+        <v>49</v>
+      </c>
+      <c r="F2" t="s">
+        <v>55</v>
+      </c>
+      <c r="H2" t="s">
+        <v>65</v>
+      </c>
+      <c r="J2" t="s">
+        <v>71</v>
+      </c>
+      <c r="K2" t="s">
+        <v>81</v>
+      </c>
+      <c r="L2" t="s">
+        <v>88</v>
+      </c>
+      <c r="M2" t="s">
+        <v>88</v>
+      </c>
+      <c r="O2" t="b">
+        <v>0</v>
+      </c>
+      <c r="P2" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q2" t="b">
+        <v>0</v>
+      </c>
+      <c r="R2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18">
+      <c r="A3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C3" t="s">
+        <v>39</v>
+      </c>
+      <c r="D3" t="s">
+        <v>48</v>
+      </c>
+      <c r="E3" t="s">
+        <v>49</v>
+      </c>
+      <c r="F3" t="s">
+        <v>56</v>
+      </c>
+      <c r="H3" t="s">
+        <v>65</v>
+      </c>
+      <c r="J3" t="s">
+        <v>72</v>
+      </c>
+      <c r="K3" t="s">
+        <v>82</v>
+      </c>
+      <c r="L3" t="s">
+        <v>89</v>
+      </c>
+      <c r="M3" t="s">
+        <v>89</v>
+      </c>
+      <c r="O3" t="b">
+        <v>0</v>
+      </c>
+      <c r="P3" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q3" t="b">
+        <v>0</v>
+      </c>
+      <c r="R3" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18">
+      <c r="A4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B4" t="s">
+        <v>30</v>
+      </c>
+      <c r="C4" t="s">
+        <v>40</v>
+      </c>
+      <c r="D4" t="s">
+        <v>48</v>
+      </c>
+      <c r="E4" t="s">
+        <v>50</v>
+      </c>
+      <c r="F4" t="s">
+        <v>57</v>
+      </c>
+      <c r="H4" t="s">
+        <v>66</v>
+      </c>
+      <c r="J4" t="s">
+        <v>73</v>
+      </c>
+      <c r="K4" t="s">
+        <v>83</v>
+      </c>
+      <c r="L4" t="s">
+        <v>90</v>
+      </c>
+      <c r="M4" t="s">
+        <v>90</v>
+      </c>
+      <c r="O4" t="b">
+        <v>0</v>
+      </c>
+      <c r="P4" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q4" t="b">
+        <v>0</v>
+      </c>
+      <c r="R4" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18">
+      <c r="A5" t="s">
+        <v>21</v>
+      </c>
+      <c r="B5" t="s">
+        <v>31</v>
+      </c>
+      <c r="C5" t="s">
+        <v>41</v>
+      </c>
+      <c r="D5" t="s">
+        <v>48</v>
+      </c>
+      <c r="E5" t="s">
+        <v>51</v>
+      </c>
+      <c r="F5" t="s">
+        <v>58</v>
+      </c>
+      <c r="H5" t="s">
+        <v>67</v>
+      </c>
+      <c r="J5" t="s">
+        <v>74</v>
+      </c>
+      <c r="K5" t="s">
+        <v>84</v>
+      </c>
+      <c r="L5" t="s">
+        <v>91</v>
+      </c>
+      <c r="M5" t="s">
+        <v>91</v>
+      </c>
+      <c r="O5" t="b">
+        <v>0</v>
+      </c>
+      <c r="P5" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q5" t="b">
+        <v>0</v>
+      </c>
+      <c r="R5" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18">
+      <c r="A6" t="s">
+        <v>22</v>
+      </c>
+      <c r="B6" t="s">
+        <v>32</v>
+      </c>
+      <c r="C6" t="s">
+        <v>42</v>
+      </c>
+      <c r="D6" t="s">
+        <v>48</v>
+      </c>
+      <c r="E6" t="s">
+        <v>51</v>
+      </c>
+      <c r="F6" t="s">
+        <v>59</v>
+      </c>
+      <c r="H6" t="s">
+        <v>67</v>
+      </c>
+      <c r="J6" t="s">
+        <v>75</v>
+      </c>
+      <c r="K6" t="s">
+        <v>82</v>
+      </c>
+      <c r="L6" t="s">
+        <v>92</v>
+      </c>
+      <c r="M6" t="s">
+        <v>92</v>
+      </c>
+      <c r="O6" t="b">
+        <v>0</v>
+      </c>
+      <c r="P6" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q6" t="b">
+        <v>0</v>
+      </c>
+      <c r="R6" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18">
+      <c r="A7" t="s">
+        <v>23</v>
+      </c>
+      <c r="B7" t="s">
+        <v>33</v>
+      </c>
+      <c r="C7" t="s">
+        <v>43</v>
+      </c>
+      <c r="D7" t="s">
+        <v>48</v>
+      </c>
+      <c r="E7" t="s">
+        <v>51</v>
+      </c>
+      <c r="F7" t="s">
+        <v>60</v>
+      </c>
+      <c r="H7" t="s">
+        <v>67</v>
+      </c>
+      <c r="J7" t="s">
+        <v>76</v>
+      </c>
+      <c r="K7" t="s">
+        <v>85</v>
+      </c>
+      <c r="L7" t="s">
+        <v>93</v>
+      </c>
+      <c r="M7" t="s">
+        <v>93</v>
+      </c>
+      <c r="O7" t="b">
+        <v>0</v>
+      </c>
+      <c r="P7" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q7" t="b">
+        <v>0</v>
+      </c>
+      <c r="R7" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18">
+      <c r="A8" t="s">
+        <v>24</v>
+      </c>
+      <c r="B8" t="s">
+        <v>34</v>
+      </c>
+      <c r="C8" t="s">
+        <v>44</v>
+      </c>
+      <c r="D8" t="s">
+        <v>48</v>
+      </c>
+      <c r="E8" t="s">
+        <v>52</v>
+      </c>
+      <c r="F8" t="s">
+        <v>61</v>
+      </c>
+      <c r="H8" t="s">
+        <v>68</v>
+      </c>
+      <c r="J8" t="s">
+        <v>77</v>
+      </c>
+      <c r="K8" t="s">
+        <v>84</v>
+      </c>
+      <c r="L8" t="s">
+        <v>94</v>
+      </c>
+      <c r="M8" t="s">
+        <v>94</v>
+      </c>
+      <c r="O8" t="b">
+        <v>0</v>
+      </c>
+      <c r="P8" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q8" t="b">
+        <v>0</v>
+      </c>
+      <c r="R8" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18">
+      <c r="A9" t="s">
+        <v>25</v>
+      </c>
+      <c r="B9" t="s">
+        <v>35</v>
+      </c>
+      <c r="C9" t="s">
+        <v>45</v>
+      </c>
+      <c r="D9" t="s">
+        <v>48</v>
+      </c>
+      <c r="E9" t="s">
+        <v>52</v>
+      </c>
+      <c r="F9" t="s">
+        <v>62</v>
+      </c>
+      <c r="H9" t="s">
+        <v>68</v>
+      </c>
+      <c r="J9" t="s">
+        <v>78</v>
+      </c>
+      <c r="K9" t="s">
+        <v>86</v>
+      </c>
+      <c r="L9" t="s">
+        <v>95</v>
+      </c>
+      <c r="M9" t="s">
+        <v>95</v>
+      </c>
+      <c r="O9" t="b">
+        <v>1</v>
+      </c>
+      <c r="P9" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q9" t="b">
+        <v>1</v>
+      </c>
+      <c r="R9" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18">
+      <c r="A10" t="s">
+        <v>26</v>
+      </c>
+      <c r="B10" t="s">
+        <v>36</v>
+      </c>
+      <c r="C10" t="s">
+        <v>46</v>
+      </c>
+      <c r="D10" t="s">
+        <v>48</v>
+      </c>
+      <c r="E10" t="s">
+        <v>53</v>
+      </c>
+      <c r="F10" t="s">
+        <v>63</v>
+      </c>
+      <c r="H10" t="s">
+        <v>69</v>
+      </c>
+      <c r="J10" t="s">
+        <v>79</v>
+      </c>
+      <c r="K10" t="s">
+        <v>87</v>
+      </c>
+      <c r="L10" t="s">
+        <v>96</v>
+      </c>
+      <c r="M10" t="s">
+        <v>96</v>
+      </c>
+      <c r="O10" t="b">
+        <v>0</v>
+      </c>
+      <c r="P10" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q10" t="b">
+        <v>0</v>
+      </c>
+      <c r="R10" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18">
+      <c r="A11" t="s">
         <v>27</v>
       </c>
-      <c r="D2" t="s">
+      <c r="B11" t="s">
         <v>37</v>
       </c>
-      <c r="E2" t="s">
-        <v>38</v>
-      </c>
-      <c r="F2" t="s">
-        <v>44</v>
-      </c>
-      <c r="G2" t="s">
+      <c r="C11" t="s">
+        <v>47</v>
+      </c>
+      <c r="D11" t="s">
+        <v>48</v>
+      </c>
+      <c r="E11" t="s">
         <v>54</v>
       </c>
-      <c r="I2" t="s">
-        <v>60</v>
-      </c>
-      <c r="J2" t="s">
+      <c r="F11" t="s">
+        <v>64</v>
+      </c>
+      <c r="H11" t="s">
         <v>70</v>
       </c>
-      <c r="N2" t="b">
-        <v>0</v>
-      </c>
-      <c r="P2" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:17">
-      <c r="A3" t="s">
-        <v>18</v>
-      </c>
-      <c r="C3" t="s">
-        <v>28</v>
-      </c>
-      <c r="D3" t="s">
-        <v>37</v>
-      </c>
-      <c r="E3" t="s">
-        <v>38</v>
-      </c>
-      <c r="F3" t="s">
-        <v>45</v>
-      </c>
-      <c r="G3" t="s">
-        <v>54</v>
-      </c>
-      <c r="I3" t="s">
-        <v>61</v>
-      </c>
-      <c r="J3" t="s">
-        <v>71</v>
-      </c>
-      <c r="N3" t="b">
-        <v>0</v>
-      </c>
-      <c r="P3" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:17">
-      <c r="A4" t="s">
-        <v>19</v>
-      </c>
-      <c r="C4" t="s">
-        <v>29</v>
-      </c>
-      <c r="D4" t="s">
-        <v>37</v>
-      </c>
-      <c r="E4" t="s">
-        <v>39</v>
-      </c>
-      <c r="F4" t="s">
-        <v>46</v>
-      </c>
-      <c r="G4" t="s">
-        <v>55</v>
-      </c>
-      <c r="I4" t="s">
-        <v>62</v>
-      </c>
-      <c r="J4" t="s">
-        <v>72</v>
-      </c>
-      <c r="N4" t="b">
-        <v>0</v>
-      </c>
-      <c r="P4" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:17">
-      <c r="A5" t="s">
-        <v>20</v>
-      </c>
-      <c r="C5" t="s">
-        <v>30</v>
-      </c>
-      <c r="D5" t="s">
-        <v>37</v>
-      </c>
-      <c r="E5" t="s">
-        <v>40</v>
-      </c>
-      <c r="F5" t="s">
-        <v>47</v>
-      </c>
-      <c r="G5" t="s">
-        <v>56</v>
-      </c>
-      <c r="I5" t="s">
-        <v>63</v>
-      </c>
-      <c r="J5" t="s">
-        <v>73</v>
-      </c>
-      <c r="N5" t="b">
-        <v>0</v>
-      </c>
-      <c r="P5" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:17">
-      <c r="A6" t="s">
-        <v>21</v>
-      </c>
-      <c r="C6" t="s">
-        <v>31</v>
-      </c>
-      <c r="D6" t="s">
-        <v>37</v>
-      </c>
-      <c r="E6" t="s">
-        <v>40</v>
-      </c>
-      <c r="F6" t="s">
-        <v>48</v>
-      </c>
-      <c r="G6" t="s">
-        <v>56</v>
-      </c>
-      <c r="I6" t="s">
-        <v>64</v>
-      </c>
-      <c r="J6" t="s">
-        <v>71</v>
-      </c>
-      <c r="N6" t="b">
-        <v>0</v>
-      </c>
-      <c r="P6" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:17">
-      <c r="A7" t="s">
-        <v>22</v>
-      </c>
-      <c r="C7" t="s">
-        <v>32</v>
-      </c>
-      <c r="D7" t="s">
-        <v>37</v>
-      </c>
-      <c r="E7" t="s">
-        <v>40</v>
-      </c>
-      <c r="F7" t="s">
-        <v>49</v>
-      </c>
-      <c r="G7" t="s">
-        <v>56</v>
-      </c>
-      <c r="I7" t="s">
-        <v>65</v>
-      </c>
-      <c r="J7" t="s">
-        <v>74</v>
-      </c>
-      <c r="N7" t="b">
-        <v>0</v>
-      </c>
-      <c r="P7" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:17">
-      <c r="A8" t="s">
-        <v>23</v>
-      </c>
-      <c r="C8" t="s">
-        <v>33</v>
-      </c>
-      <c r="D8" t="s">
-        <v>37</v>
-      </c>
-      <c r="E8" t="s">
-        <v>41</v>
-      </c>
-      <c r="F8" t="s">
-        <v>50</v>
-      </c>
-      <c r="G8" t="s">
-        <v>57</v>
-      </c>
-      <c r="I8" t="s">
-        <v>66</v>
-      </c>
-      <c r="J8" t="s">
-        <v>73</v>
-      </c>
-      <c r="N8" t="b">
-        <v>0</v>
-      </c>
-      <c r="P8" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:17">
-      <c r="A9" t="s">
-        <v>24</v>
-      </c>
-      <c r="C9" t="s">
-        <v>34</v>
-      </c>
-      <c r="D9" t="s">
-        <v>37</v>
-      </c>
-      <c r="E9" t="s">
-        <v>41</v>
-      </c>
-      <c r="F9" t="s">
-        <v>51</v>
-      </c>
-      <c r="G9" t="s">
-        <v>57</v>
-      </c>
-      <c r="I9" t="s">
-        <v>67</v>
-      </c>
-      <c r="J9" t="s">
-        <v>75</v>
-      </c>
-      <c r="N9" t="b">
-        <v>1</v>
-      </c>
-      <c r="P9" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:17">
-      <c r="A10" t="s">
-        <v>25</v>
-      </c>
-      <c r="C10" t="s">
-        <v>35</v>
-      </c>
-      <c r="D10" t="s">
-        <v>37</v>
-      </c>
-      <c r="E10" t="s">
-        <v>42</v>
-      </c>
-      <c r="F10" t="s">
-        <v>52</v>
-      </c>
-      <c r="G10" t="s">
-        <v>58</v>
-      </c>
-      <c r="I10" t="s">
-        <v>68</v>
-      </c>
-      <c r="J10" t="s">
-        <v>76</v>
-      </c>
-      <c r="N10" t="b">
-        <v>0</v>
-      </c>
-      <c r="P10" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:17">
-      <c r="A11" t="s">
-        <v>26</v>
-      </c>
-      <c r="C11" t="s">
-        <v>36</v>
-      </c>
-      <c r="D11" t="s">
-        <v>37</v>
-      </c>
-      <c r="E11" t="s">
-        <v>43</v>
-      </c>
-      <c r="F11" t="s">
-        <v>53</v>
-      </c>
-      <c r="G11" t="s">
-        <v>59</v>
-      </c>
-      <c r="I11" t="s">
-        <v>69</v>
-      </c>
       <c r="J11" t="s">
-        <v>71</v>
-      </c>
-      <c r="N11" t="b">
+        <v>80</v>
+      </c>
+      <c r="K11" t="s">
+        <v>82</v>
+      </c>
+      <c r="L11" t="s">
+        <v>97</v>
+      </c>
+      <c r="M11" t="s">
+        <v>97</v>
+      </c>
+      <c r="O11" t="b">
         <v>0</v>
       </c>
       <c r="P11" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q11" t="b">
+        <v>0</v>
+      </c>
+      <c r="R11" t="b">
         <v>0</v>
       </c>
     </row>

</xml_diff>